<commit_message>
added changes to better shoosing players
</commit_message>
<xml_diff>
--- a/sorare/anton.xlsx
+++ b/sorare/anton.xlsx
@@ -79,9 +79,6 @@
     <t xml:space="preserve">CRISTIAN BRAUN</t>
   </si>
   <si>
-    <t xml:space="preserve">MOUSSA DIABATE</t>
-  </si>
-  <si>
     <t xml:space="preserve">DEVONTE GRAHAM</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t xml:space="preserve">MARK WILLIAMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRED VANVLEET</t>
   </si>
 </sst>
 </file>
@@ -199,7 +199,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -223,10 +223,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,7 +237,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -259,7 +259,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +270,7 @@
         <v>39</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,10 +278,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -289,10 +289,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,7 +303,7 @@
         <v>27</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -311,10 +311,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -325,7 +325,7 @@
         <v>24</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -333,10 +333,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="1" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -344,10 +344,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -355,10 +355,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,10 +366,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,21 +399,21 @@
         <v>19</v>
       </c>
       <c r="B18" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="C18" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C18" s="1" t="n">
-        <v>4</v>
-      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +424,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="0" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,7 +435,7 @@
         <v>7</v>
       </c>
       <c r="C21" s="0" t="n">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,10 +443,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="0" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="0" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -454,10 +454,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="0" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="C23" s="0" t="n">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>